<commit_message>
EditAccount Test Commit to MyBranch
</commit_message>
<xml_diff>
--- a/inetBankingV1/src/test/java/com/inetbanking/testData/LoginData.xlsx
+++ b/inetBankingV1/src/test/java/com/inetbanking/testData/LoginData.xlsx
@@ -87,7 +87,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -110,14 +110,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +444,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -476,6 +488,9 @@
         <v>5</v>
       </c>
     </row>
+    <row r="5" spans="1:2" ht="23.4">
+      <c r="B5" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>